<commit_message>
feat : RobotConfig fix on strategy not used, manage Small Robot perimeter problem (left and right up), big Robot release in two phase, manage distance for side Tof
</commit_message>
<xml_diff>
--- a/documentation/matchProcedures.xlsx
+++ b/documentation/matchProcedures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\cen-electronic\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\svanacker\cen-electronic\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E752876-6345-4D13-9529-AEA55C2536A6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A42F5-FB73-409B-9E58-85A5FA662DF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{6F9D2041-9D74-4F50-8EFC-DF9BCD1711A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{6F9D2041-9D74-4F50-8EFC-DF9BCD1711A6}"/>
   </bookViews>
   <sheets>
     <sheet name="CHECKLIST VOYAGE" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
   <si>
     <t>Mettre la tirette</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>PLAYER 1</t>
-  </si>
-  <si>
-    <t>Vérifier le positionnement du distributeur (vertical)</t>
   </si>
   <si>
     <t>Obtenir la couleur</t>
@@ -81,12 +78,6 @@
     <t>Récupérer la tirette</t>
   </si>
   <si>
-    <t>Récupérer la balise Catadioptre</t>
-  </si>
-  <si>
-    <t>Récupérer le Robot</t>
-  </si>
-  <si>
     <t>Récupérer l'Abeille</t>
   </si>
   <si>
@@ -119,9 +110,6 @@
 GREEN ou ORANGE</t>
   </si>
   <si>
-    <t>Vérifier qu'il n'y a pas de balles à l'intérieur du distributeur</t>
-  </si>
-  <si>
     <t>Batteries 9V</t>
   </si>
   <si>
@@ -318,6 +306,9 @@
   </si>
   <si>
     <t>Vérifier la configuration en dehors de la couleur</t>
+  </si>
+  <si>
+    <t>Récupérer le Robot 1</t>
   </si>
 </sst>
 </file>
@@ -610,35 +601,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -685,6 +652,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,7 +695,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1002,128 +993,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E580376-F827-4668-A8C6-F2EDA2AFF9A5}">
   <dimension ref="A2:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1136,10 +1127,10 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
@@ -1148,192 +1139,192 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1349,84 +1340,84 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1442,29 +1433,29 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1476,298 +1467,288 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6354E8C8-36D5-4265-BDB2-55D04B5C92AE}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="A2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="3">
         <v>10</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="35">
+      <c r="A3" s="11"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
         <v>10</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B6" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="C6" s="4"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
         <v>10</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="18"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <v>10</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="18"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>10</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="18"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="30">
+      <c r="A8" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="22">
         <v>30</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B15" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="C15" s="4"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>20</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3">
+        <v>20</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2">
+        <v>60</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
         <v>10</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="7">
-        <v>10</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4">
-        <v>20</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="7">
-        <v>20</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="4">
-        <v>60</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="7">
-        <v>20</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="23"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="4">
-        <v>20</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="7">
-        <v>20</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="23"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="4">
-        <v>10</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="3"/>
+      <c r="A24" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="29"/>
       <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="18"/>
-    </row>
-    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="B28" s="35"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="18"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="18"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="18"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;CFOCUS ROBOTIQUE 2018</oddHeader>
     <oddFooter>&amp;A</oddFooter>

</xml_diff>